<commit_message>
updates to hookregNL some citation added Table about data updated
</commit_message>
<xml_diff>
--- a/inst/Table_human_rated.xlsx
+++ b/inst/Table_human_rated.xlsx
@@ -16,6 +16,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">_!$A$1:$H$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="110">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -296,10 +297,25 @@
     <t xml:space="preserve">F09~WGA</t>
   </si>
   <si>
+    <t xml:space="preserve">Evrogen lab experiment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whole genome amplification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EvaGreen</t>
+  </si>
+  <si>
     <t xml:space="preserve">F10~WGA</t>
   </si>
   <si>
     <t xml:space="preserve">F11~1ng/mkl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRCA1 gene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TaqMan (HEX/BHQ1)</t>
   </si>
   <si>
     <t xml:space="preserve">F12~1ng/mkl</t>
@@ -508,8 +524,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="C82" colorId="64" zoomScale="160" zoomScaleNormal="100" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H88" activeCellId="0" sqref="H88"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D76" activeCellId="0" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2329,6 +2345,15 @@
       <c r="B70" s="9" t="s">
         <v>87</v>
       </c>
+      <c r="C70" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="F70" s="6" t="s">
         <v>12</v>
       </c>
@@ -2344,7 +2369,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>88</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>12</v>
@@ -2361,9 +2395,17 @@
         <v>71</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E72" s="0"/>
+        <v>92</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F72" s="6" t="s">
         <v>12</v>
       </c>
@@ -2379,9 +2421,17 @@
         <v>72</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E73" s="0"/>
+        <v>95</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F73" s="6" t="s">
         <v>12</v>
       </c>
@@ -2397,7 +2447,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>91</v>
+        <v>96</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>12</v>
@@ -2414,7 +2473,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>92</v>
+        <v>97</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>12</v>
@@ -2431,9 +2499,17 @@
         <v>75</v>
       </c>
       <c r="B76" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E76" s="0"/>
+      <c r="E76" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F76" s="6" t="s">
         <v>17</v>
       </c>
@@ -2449,9 +2525,17 @@
         <v>76</v>
       </c>
       <c r="B77" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E77" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E77" s="0"/>
       <c r="F77" s="6" t="s">
         <v>17</v>
       </c>
@@ -2467,7 +2551,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>95</v>
+        <v>100</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>17</v>
@@ -2484,7 +2577,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>96</v>
+        <v>101</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>17</v>
@@ -2501,9 +2603,17 @@
         <v>79</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E80" s="0"/>
+        <v>102</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F80" s="6" t="s">
         <v>12</v>
       </c>
@@ -2519,9 +2629,17 @@
         <v>80</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="E81" s="0"/>
+        <v>103</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F81" s="6" t="s">
         <v>12</v>
       </c>
@@ -2537,7 +2655,16 @@
         <v>81</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>99</v>
+        <v>104</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>12</v>
@@ -2554,7 +2681,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>100</v>
+        <v>105</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>12</v>
@@ -2571,9 +2707,17 @@
         <v>83</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E84" s="0"/>
+        <v>106</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F84" s="6" t="s">
         <v>17</v>
       </c>
@@ -2589,9 +2733,17 @@
         <v>84</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E85" s="0"/>
+        <v>107</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F85" s="6" t="s">
         <v>17</v>
       </c>
@@ -2607,7 +2759,16 @@
         <v>85</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>103</v>
+        <v>108</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>17</v>
@@ -2624,11 +2785,17 @@
         <v>86</v>
       </c>
       <c r="B87" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-      <c r="E87" s="10"/>
+        <v>109</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="F87" s="6" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
updated table and documentation
</commit_message>
<xml_diff>
--- a/inst/Table_human_rated.xlsx
+++ b/inst/Table_human_rated.xlsx
@@ -11,15 +11,16 @@
     <sheet name="_" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">_!$A$1:$H$97</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">_!$A$1:$H$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">_!$A$1:$H$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">_!$A$1:$H$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">_!$A$1:$H$95</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">_!$A$1:$H$87</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="119">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -388,6 +389,9 @@
   </si>
   <si>
     <t xml:space="preserve">s8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NTC</t>
   </si>
 </sst>
 </file>
@@ -545,10 +549,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ95"/>
+  <dimension ref="A1:AMJ97"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A66" colorId="64" zoomScale="130" zoomScaleNormal="100" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H94" activeCellId="0" sqref="H94"/>
+      <selection pane="topLeft" activeCell="B98" activeCellId="0" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3037,10 +3041,62 @@
         <v>1</v>
       </c>
     </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="10" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G96" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H96" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="10" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="53" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="52" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>